<commit_message>
Added methods for ExcelSubTable interface Added mockito dependency
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelExample.xlsx
+++ b/src/test/resources/ExcelExample.xlsx
@@ -14,42 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Шапка1</t>
-  </si>
-  <si>
-    <t>Шапка2</t>
-  </si>
-  <si>
-    <t>Шапка3</t>
-  </si>
-  <si>
-    <t>Шапка4</t>
-  </si>
-  <si>
-    <t>Дата1</t>
-  </si>
-  <si>
-    <t>Дата2</t>
-  </si>
-  <si>
-    <t>Дата3</t>
-  </si>
-  <si>
-    <t>Дата4</t>
-  </si>
-  <si>
-    <t>Строка</t>
-  </si>
-  <si>
-    <t>Опять строка</t>
-  </si>
-  <si>
-    <t>Первая ячейка</t>
-  </si>
-  <si>
-    <t>Пам-пам</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>First Cell</t>
+  </si>
+  <si>
+    <t>Foo</t>
+  </si>
+  <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>Header1</t>
+  </si>
+  <si>
+    <t>Header2</t>
+  </si>
+  <si>
+    <t>Header3</t>
+  </si>
+  <si>
+    <t>Header4</t>
+  </si>
+  <si>
+    <t>Bas</t>
   </si>
 </sst>
 </file>
@@ -394,49 +391,49 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I6" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>123</v>
       </c>
       <c r="I7" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <v>456</v>
@@ -444,15 +441,15 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H10">
         <v>789</v>

</xml_diff>